<commit_message>
horrible giant bad commit
Signed-off-by: ahoetker <ahoetker@me.com>
</commit_message>
<xml_diff>
--- a/tests/resources/input_table.xlsx
+++ b/tests/resources/input_table.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Heat Capacity Flowrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Enthalpy</t>
+    <t xml:space="preserve">Heat Flow</t>
   </si>
   <si>
     <t xml:space="preserve">degC</t>
@@ -82,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,12 +170,12 @@
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.33"/>
   </cols>
   <sheetData>
@@ -229,7 +230,7 @@
         <v>101.2</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>41605.3</v>
+        <v>41605.344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,7 +250,7 @@
         <v>102</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>59155.9</v>
+        <v>59155.92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,7 +310,7 @@
         <v>597</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>15259.3</v>
+        <v>15259.32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +330,7 @@
         <v>216</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>-103654.1</v>
+        <v>-103654.08</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>